<commit_message>
Adding Dan Hentschel's comments
</commit_message>
<xml_diff>
--- a/VectorRegisters.xlsx
+++ b/VectorRegisters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13740" windowHeight="4800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="39">
   <si>
     <t>B</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>mask</t>
+  </si>
+  <si>
+    <t>value_true</t>
+  </si>
+  <si>
+    <t>value_false</t>
+  </si>
+  <si>
+    <t>result</t>
   </si>
 </sst>
 </file>
@@ -315,13 +327,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -333,6 +345,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -342,21 +363,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -491,6 +508,1066 @@
               <a:schemeClr val="tx1"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Igual que 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3895725" y="3209925"/>
+          <a:ext cx="495300" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathEqual">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Multiplicar 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1390650" y="2428875"/>
+          <a:ext cx="447675" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="60000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Multiplicar 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2114550" y="2438400"/>
+          <a:ext cx="447675" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="60000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Multiplicar 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2828925" y="2419350"/>
+          <a:ext cx="447675" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="60000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>400050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Flecha abajo 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1504950" y="3171825"/>
+          <a:ext cx="257175" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>400050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Flecha abajo 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2200275" y="3171825"/>
+          <a:ext cx="257175" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>400050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Flecha abajo 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2952750" y="3171825"/>
+          <a:ext cx="257175" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Multiplicar 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3562350" y="2857500"/>
+          <a:ext cx="447675" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="60000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Multiplicar 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4295775" y="2838450"/>
+          <a:ext cx="447675" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="60000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Multiplicar 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5010150" y="2828925"/>
+          <a:ext cx="447675" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="60000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Multiplicar 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5705475" y="2838450"/>
+          <a:ext cx="447675" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="60000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Multiplicar 16"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6477000" y="2828925"/>
+          <a:ext cx="447675" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="60000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>400050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Flecha abajo 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3667126" y="2752725"/>
+          <a:ext cx="266700" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>400050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Flecha abajo 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4381500" y="2752725"/>
+          <a:ext cx="266700" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>400050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Flecha abajo 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5114925" y="2752725"/>
+          <a:ext cx="266700" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Flecha abajo 20"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5819775" y="2743200"/>
+          <a:ext cx="266700" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Flecha abajo 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6553200" y="2743200"/>
+          <a:ext cx="266700" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1160,12 +2237,22 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="AF6:AM6"/>
-    <mergeCell ref="X6:AE6"/>
-    <mergeCell ref="X4:AA4"/>
-    <mergeCell ref="AB4:AE4"/>
-    <mergeCell ref="AF4:AI4"/>
-    <mergeCell ref="AJ4:AM4"/>
+    <mergeCell ref="AJ20:AM20"/>
+    <mergeCell ref="X16:AM16"/>
+    <mergeCell ref="X22:AE22"/>
+    <mergeCell ref="AF22:AM22"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="P20:S20"/>
+    <mergeCell ref="T20:W20"/>
+    <mergeCell ref="X20:AA20"/>
+    <mergeCell ref="H22:O22"/>
+    <mergeCell ref="P22:W22"/>
+    <mergeCell ref="X12:AA12"/>
+    <mergeCell ref="AB12:AE12"/>
+    <mergeCell ref="AF12:AI12"/>
+    <mergeCell ref="AB20:AE20"/>
+    <mergeCell ref="AF20:AI20"/>
     <mergeCell ref="AJ12:AM12"/>
     <mergeCell ref="X14:AE14"/>
     <mergeCell ref="AF14:AM14"/>
@@ -1177,22 +2264,12 @@
     <mergeCell ref="AD10:AE10"/>
     <mergeCell ref="AF10:AG10"/>
     <mergeCell ref="AH10:AI10"/>
-    <mergeCell ref="H22:O22"/>
-    <mergeCell ref="P22:W22"/>
-    <mergeCell ref="X12:AA12"/>
-    <mergeCell ref="AB12:AE12"/>
-    <mergeCell ref="AF12:AI12"/>
-    <mergeCell ref="AB20:AE20"/>
-    <mergeCell ref="AF20:AI20"/>
-    <mergeCell ref="AJ20:AM20"/>
-    <mergeCell ref="X16:AM16"/>
-    <mergeCell ref="X22:AE22"/>
-    <mergeCell ref="AF22:AM22"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="P20:S20"/>
-    <mergeCell ref="T20:W20"/>
-    <mergeCell ref="X20:AA20"/>
+    <mergeCell ref="AF6:AM6"/>
+    <mergeCell ref="X6:AE6"/>
+    <mergeCell ref="X4:AA4"/>
+    <mergeCell ref="AB4:AE4"/>
+    <mergeCell ref="AF4:AI4"/>
+    <mergeCell ref="AJ4:AM4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1200,10 +2277,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F1:AM8"/>
+  <dimension ref="F1:AM18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="AK32" sqref="AK32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,54 +2297,54 @@
       <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="11" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="11" t="s">
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="11" t="s">
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="11" t="s">
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="11" t="s">
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="11" t="s">
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="11" t="s">
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="19"/>
+      <c r="AJ2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
-      <c r="AM2" s="13"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="19"/>
     </row>
     <row r="3" spans="6:39" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="6:39" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1275,54 +2352,54 @@
       <c r="F5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="17" t="s">
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="17" t="s">
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="17" t="s">
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="17" t="s">
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="18"/>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="17" t="s">
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="AC5" s="18"/>
-      <c r="AD5" s="18"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="17" t="s">
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="21"/>
+      <c r="AE5" s="22"/>
+      <c r="AF5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="AG5" s="18"/>
-      <c r="AH5" s="18"/>
-      <c r="AI5" s="19"/>
-      <c r="AJ5" s="17" t="s">
+      <c r="AG5" s="21"/>
+      <c r="AH5" s="21"/>
+      <c r="AI5" s="22"/>
+      <c r="AJ5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="AK5" s="18"/>
-      <c r="AL5" s="18"/>
-      <c r="AM5" s="19"/>
+      <c r="AK5" s="21"/>
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="22"/>
     </row>
     <row r="7" spans="6:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="6:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1347,47 +2424,287 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="16"/>
-      <c r="T8" s="20" t="s">
+      <c r="T8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="22"/>
-      <c r="X8" s="20" t="s">
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="22"/>
-      <c r="AB8" s="20" t="s">
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21"/>
-      <c r="AE8" s="22"/>
-      <c r="AF8" s="20" t="s">
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AG8" s="21"/>
-      <c r="AH8" s="21"/>
-      <c r="AI8" s="22"/>
-      <c r="AJ8" s="20" t="s">
+      <c r="AG8" s="12"/>
+      <c r="AH8" s="12"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AK8" s="21"/>
-      <c r="AL8" s="21"/>
-      <c r="AM8" s="22"/>
+      <c r="AK8" s="12"/>
+      <c r="AL8" s="12"/>
+      <c r="AM8" s="13"/>
+    </row>
+    <row r="11" spans="6:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="6:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC12" s="12"/>
+      <c r="AD12" s="12"/>
+      <c r="AE12" s="13"/>
+      <c r="AF12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG12" s="12"/>
+      <c r="AH12" s="12"/>
+      <c r="AI12" s="13"/>
+      <c r="AJ12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK12" s="12"/>
+      <c r="AL12" s="12"/>
+      <c r="AM12" s="13"/>
+    </row>
+    <row r="13" spans="6:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="6:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="18"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC14" s="18"/>
+      <c r="AD14" s="18"/>
+      <c r="AE14" s="19"/>
+      <c r="AF14" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG14" s="18"/>
+      <c r="AH14" s="18"/>
+      <c r="AI14" s="19"/>
+      <c r="AJ14" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK14" s="18"/>
+      <c r="AL14" s="18"/>
+      <c r="AM14" s="19"/>
+    </row>
+    <row r="15" spans="6:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="6:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="U16" s="21"/>
+      <c r="V16" s="21"/>
+      <c r="W16" s="22"/>
+      <c r="X16" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="21"/>
+      <c r="AA16" s="22"/>
+      <c r="AB16" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC16" s="21"/>
+      <c r="AD16" s="21"/>
+      <c r="AE16" s="22"/>
+      <c r="AF16" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG16" s="21"/>
+      <c r="AH16" s="21"/>
+      <c r="AI16" s="22"/>
+      <c r="AJ16" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK16" s="21"/>
+      <c r="AL16" s="21"/>
+      <c r="AM16" s="22"/>
+    </row>
+    <row r="17" spans="6:39" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="6:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="U18" s="21"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y18" s="21"/>
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="22"/>
+      <c r="AB18" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC18" s="21"/>
+      <c r="AD18" s="21"/>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG18" s="21"/>
+      <c r="AH18" s="21"/>
+      <c r="AI18" s="22"/>
+      <c r="AJ18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK18" s="21"/>
+      <c r="AL18" s="21"/>
+      <c r="AM18" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="AF8:AI8"/>
-    <mergeCell ref="AJ8:AM8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="X8:AA8"/>
-    <mergeCell ref="AB8:AE8"/>
+  <mergeCells count="56">
+    <mergeCell ref="AB18:AE18"/>
+    <mergeCell ref="AF18:AI18"/>
+    <mergeCell ref="AJ18:AM18"/>
+    <mergeCell ref="AB12:AE12"/>
+    <mergeCell ref="AF12:AI12"/>
+    <mergeCell ref="AJ12:AM12"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="P18:S18"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="X18:AA18"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="T12:W12"/>
+    <mergeCell ref="X12:AA12"/>
+    <mergeCell ref="AB14:AE14"/>
+    <mergeCell ref="AF14:AI14"/>
+    <mergeCell ref="AJ14:AM14"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="P16:S16"/>
+    <mergeCell ref="T16:W16"/>
+    <mergeCell ref="X16:AA16"/>
+    <mergeCell ref="AB16:AE16"/>
+    <mergeCell ref="AF16:AI16"/>
+    <mergeCell ref="AJ16:AM16"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="T14:W14"/>
+    <mergeCell ref="X14:AA14"/>
     <mergeCell ref="AJ2:AM2"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="L5:O5"/>
@@ -1404,6 +2721,14 @@
     <mergeCell ref="AB5:AE5"/>
     <mergeCell ref="AF5:AI5"/>
     <mergeCell ref="AJ5:AM5"/>
+    <mergeCell ref="AF8:AI8"/>
+    <mergeCell ref="AJ8:AM8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="X8:AA8"/>
+    <mergeCell ref="AB8:AE8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>